<commit_message>
Output Missing Files File
</commit_message>
<xml_diff>
--- a/missing_files_report.xlsx
+++ b/missing_files_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +440,20 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>IB User with blank Card via EBS (Tagged to Credit Card Brn) at at -12-Dec-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Active IB User of at -12-Dec-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
minor edit to compare
</commit_message>
<xml_diff>
--- a/missing_files_report.xlsx
+++ b/missing_files_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,12 +443,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IB User with blank Card via EBS (Tagged to Credit Card Brn) at at -12-Dec-2024</t>
+          <t>IB USer Demographic as at at -12-Dec-2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
+        <is>
+          <t>IB User with blank Card via EBS (Tagged to Credit Card Brn) at at -12-Dec-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Active IB User of at -12-Dec-2024</t>
         </is>

</xml_diff>